<commit_message>
ng: update tas forms
</commit_message>
<xml_diff>
--- a/LF/TAS/Nigeria/2024/june_2024/Kebbi/ng_lf_tas_2406_1_sit_part_kb.xlsx
+++ b/LF/TAS/Nigeria/2024/june_2024/Kebbi/ng_lf_tas_2406_1_sit_part_kb.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bonhe\Repositories\dsa-forms\LF\TAS\Nigeria\2024\june_2024\Kebbi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF9BA34D-37A2-4002-9106-8A626EA40F04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C13734E-B088-4B54-849D-6645C2207912}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -2450,15 +2450,6 @@
     <t>QUR ANIC MODEL SCHOOL</t>
   </si>
   <si>
-    <t>(June 2024) - 1. Kebbi - TAS1 LF Site &amp; participant Form V3</t>
-  </si>
-  <si>
-    <t>ng_lf_tas_2406_1_sit_part_kb_v3</t>
-  </si>
-  <si>
-    <t>ng_tas_p_2406_kb_3</t>
-  </si>
-  <si>
     <t>11</t>
   </si>
   <si>
@@ -2499,6 +2490,15 @@
   </si>
   <si>
     <t>${c_has_water} = 'Yes'</t>
+  </si>
+  <si>
+    <t>ng_tas_p_2406_kb_31</t>
+  </si>
+  <si>
+    <t>ng_lf_tas_2406_1_sit_part_kb_v31</t>
+  </si>
+  <si>
+    <t>(June 2024) Kebbi - 1. TAS1 LF Site &amp; participant Form V3</t>
   </si>
 </sst>
 </file>
@@ -3115,7 +3115,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A13" sqref="A13:XFD18"/>
+      <selection pane="bottomRight" activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3522,7 +3522,7 @@
       <c r="E16" s="6"/>
       <c r="G16" s="6"/>
       <c r="H16" s="4" t="s">
-        <v>817</v>
+        <v>814</v>
       </c>
       <c r="I16" s="6"/>
       <c r="J16" s="6" t="s">
@@ -3537,7 +3537,7 @@
         <v>26</v>
       </c>
       <c r="B17" s="36" t="s">
-        <v>818</v>
+        <v>815</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>798</v>
@@ -3570,7 +3570,7 @@
       <c r="E18" s="6"/>
       <c r="G18" s="6"/>
       <c r="H18" s="4" t="s">
-        <v>819</v>
+        <v>816</v>
       </c>
       <c r="I18" s="6"/>
       <c r="J18" s="6" t="s">
@@ -3643,7 +3643,7 @@
         <v>81</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>805</v>
+        <v>817</v>
       </c>
       <c r="C22" s="18" t="s">
         <v>82</v>
@@ -3933,7 +3933,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F1179"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A461" sqref="A461:XFD468"/>
     </sheetView>
@@ -4081,10 +4081,10 @@
         <v>69</v>
       </c>
       <c r="B12" s="27" t="s">
-        <v>806</v>
+        <v>803</v>
       </c>
       <c r="C12" s="27" t="s">
-        <v>806</v>
+        <v>803</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="4" customFormat="1">
@@ -4092,10 +4092,10 @@
         <v>69</v>
       </c>
       <c r="B13" s="27" t="s">
-        <v>807</v>
+        <v>804</v>
       </c>
       <c r="C13" s="27" t="s">
-        <v>807</v>
+        <v>804</v>
       </c>
     </row>
     <row r="14" spans="1:6" s="4" customFormat="1">
@@ -4103,10 +4103,10 @@
         <v>69</v>
       </c>
       <c r="B14" s="27" t="s">
-        <v>808</v>
+        <v>805</v>
       </c>
       <c r="C14" s="27" t="s">
-        <v>808</v>
+        <v>805</v>
       </c>
     </row>
     <row r="15" spans="1:6" s="4" customFormat="1">
@@ -4114,10 +4114,10 @@
         <v>69</v>
       </c>
       <c r="B15" s="27" t="s">
-        <v>809</v>
+        <v>806</v>
       </c>
       <c r="C15" s="27" t="s">
-        <v>809</v>
+        <v>806</v>
       </c>
     </row>
     <row r="16" spans="1:6" s="4" customFormat="1">
@@ -4125,10 +4125,10 @@
         <v>69</v>
       </c>
       <c r="B16" s="27" t="s">
-        <v>810</v>
+        <v>807</v>
       </c>
       <c r="C16" s="27" t="s">
-        <v>810</v>
+        <v>807</v>
       </c>
     </row>
     <row r="17" spans="1:6" s="4" customFormat="1">
@@ -4136,10 +4136,10 @@
         <v>69</v>
       </c>
       <c r="B17" s="27" t="s">
-        <v>811</v>
+        <v>808</v>
       </c>
       <c r="C17" s="27" t="s">
-        <v>811</v>
+        <v>808</v>
       </c>
     </row>
     <row r="18" spans="1:6" s="4" customFormat="1">
@@ -4147,10 +4147,10 @@
         <v>69</v>
       </c>
       <c r="B18" s="27" t="s">
-        <v>812</v>
+        <v>809</v>
       </c>
       <c r="C18" s="27" t="s">
-        <v>812</v>
+        <v>809</v>
       </c>
     </row>
     <row r="19" spans="1:6" s="4" customFormat="1">
@@ -4158,10 +4158,10 @@
         <v>69</v>
       </c>
       <c r="B19" s="27" t="s">
-        <v>813</v>
+        <v>810</v>
       </c>
       <c r="C19" s="27" t="s">
-        <v>813</v>
+        <v>810</v>
       </c>
     </row>
     <row r="20" spans="1:6" s="4" customFormat="1">
@@ -4169,10 +4169,10 @@
         <v>69</v>
       </c>
       <c r="B20" s="27" t="s">
-        <v>814</v>
+        <v>811</v>
       </c>
       <c r="C20" s="27" t="s">
-        <v>814</v>
+        <v>811</v>
       </c>
     </row>
     <row r="21" spans="1:6" s="4" customFormat="1">
@@ -4180,10 +4180,10 @@
         <v>69</v>
       </c>
       <c r="B21" s="27" t="s">
-        <v>815</v>
+        <v>812</v>
       </c>
       <c r="C21" s="27" t="s">
-        <v>815</v>
+        <v>812</v>
       </c>
     </row>
     <row r="22" spans="1:6" s="4" customFormat="1">
@@ -9997,10 +9997,10 @@
         <v>157</v>
       </c>
       <c r="B449" s="4" t="s">
-        <v>816</v>
+        <v>813</v>
       </c>
       <c r="C449" s="4" t="s">
-        <v>816</v>
+        <v>813</v>
       </c>
       <c r="E449" s="3" t="s">
         <v>779</v>
@@ -10011,10 +10011,10 @@
         <v>157</v>
       </c>
       <c r="B450" s="4" t="s">
-        <v>816</v>
+        <v>813</v>
       </c>
       <c r="C450" s="4" t="s">
-        <v>816</v>
+        <v>813</v>
       </c>
       <c r="E450" s="3" t="s">
         <v>780</v>
@@ -10025,10 +10025,10 @@
         <v>157</v>
       </c>
       <c r="B451" s="4" t="s">
-        <v>816</v>
+        <v>813</v>
       </c>
       <c r="C451" s="4" t="s">
-        <v>816</v>
+        <v>813</v>
       </c>
       <c r="E451" s="3" t="s">
         <v>276</v>
@@ -10039,10 +10039,10 @@
         <v>157</v>
       </c>
       <c r="B452" s="4" t="s">
-        <v>816</v>
+        <v>813</v>
       </c>
       <c r="C452" s="4" t="s">
-        <v>816</v>
+        <v>813</v>
       </c>
       <c r="E452" s="3" t="s">
         <v>782</v>
@@ -10053,10 +10053,10 @@
         <v>157</v>
       </c>
       <c r="B453" s="4" t="s">
-        <v>816</v>
+        <v>813</v>
       </c>
       <c r="C453" s="4" t="s">
-        <v>816</v>
+        <v>813</v>
       </c>
       <c r="E453" s="3" t="s">
         <v>783</v>
@@ -10067,10 +10067,10 @@
         <v>157</v>
       </c>
       <c r="B454" s="4" t="s">
-        <v>816</v>
+        <v>813</v>
       </c>
       <c r="C454" s="4" t="s">
-        <v>816</v>
+        <v>813</v>
       </c>
       <c r="E454" s="3" t="s">
         <v>781</v>
@@ -10081,10 +10081,10 @@
         <v>157</v>
       </c>
       <c r="B455" s="4" t="s">
-        <v>816</v>
+        <v>813</v>
       </c>
       <c r="C455" s="4" t="s">
-        <v>816</v>
+        <v>813</v>
       </c>
       <c r="E455" s="3" t="s">
         <v>394</v>
@@ -10095,10 +10095,10 @@
         <v>157</v>
       </c>
       <c r="B456" s="4" t="s">
-        <v>816</v>
+        <v>813</v>
       </c>
       <c r="C456" s="4" t="s">
-        <v>816</v>
+        <v>813</v>
       </c>
       <c r="E456" s="3" t="s">
         <v>785</v>
@@ -10109,10 +10109,10 @@
         <v>157</v>
       </c>
       <c r="B457" s="4" t="s">
-        <v>816</v>
+        <v>813</v>
       </c>
       <c r="C457" s="4" t="s">
-        <v>816</v>
+        <v>813</v>
       </c>
       <c r="E457" s="3" t="s">
         <v>491</v>
@@ -10123,10 +10123,10 @@
         <v>157</v>
       </c>
       <c r="B458" s="4" t="s">
-        <v>816</v>
+        <v>813</v>
       </c>
       <c r="C458" s="4" t="s">
-        <v>816</v>
+        <v>813</v>
       </c>
       <c r="E458" s="3" t="s">
         <v>784</v>
@@ -10137,10 +10137,10 @@
         <v>157</v>
       </c>
       <c r="B459" s="4" t="s">
-        <v>816</v>
+        <v>813</v>
       </c>
       <c r="C459" s="4" t="s">
-        <v>816</v>
+        <v>813</v>
       </c>
       <c r="E459" s="3" t="s">
         <v>786</v>
@@ -20213,8 +20213,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -20241,10 +20241,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="4" t="s">
-        <v>803</v>
+        <v>819</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>804</v>
+        <v>818</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>51</v>

</xml_diff>